<commit_message>
Add TODO comment in wef.R
</commit_message>
<xml_diff>
--- a/data/sources.xlsx
+++ b/data/sources.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -181,15 +181,18 @@
     <t xml:space="preserve">Global Competitiveness Index </t>
   </si>
   <si>
+    <t xml:space="preserve">not using</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laws_relating_to_icts.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laws relating to ICTs</t>
+  </si>
+  <si>
     <t xml:space="preserve">wef.R</t>
   </si>
   <si>
-    <t xml:space="preserve">laws_relating_to_icts.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laws relating to ICTs</t>
-  </si>
-  <si>
     <t xml:space="preserve">WEF_NRI_2012-2016_Historical_Dataset.xlsx</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">Global Payment Systems Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wb.R</t>
   </si>
   <si>
     <t xml:space="preserve">Global Findex Database.xlsx</t>
@@ -325,7 +331,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -585,54 +591,60 @@
         <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>

</xml_diff>